<commit_message>
No longer use excel headings
Just relies on column indices

Co-Authored-By: Jia Tee <73531134+JJTee@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/SocialMediaAnalysis/Output/inputData.xlsx
+++ b/SocialMediaAnalysis/Output/inputData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoa-my.sharepoint.com/personal/xzha897_uoa_auckland_ac_nz/Documents/Documents/GitHub/social-media-analysis/SocialMediaAnalysis/Output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="143" documentId="13_ncr:1_{E8349CB7-9F47-4A4E-BEEF-F1265ACB3467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{475952C3-C3A2-4C2E-87D5-E572CB466A35}"/>
+  <xr:revisionPtr revIDLastSave="446" documentId="13_ncr:1_{E8349CB7-9F47-4A4E-BEEF-F1265ACB3467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FED3B663-4209-4DD9-BD09-EC7169138DCD}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,39 +25,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="44">
   <si>
     <t>Tuco was actually pretty cool when he wasn’t tweaked out. As soon as he snorted he became an animal</t>
   </si>
   <si>
-    <t>Result</t>
-  </si>
-  <si>
-    <t>Sentiment</t>
-  </si>
-  <si>
-    <t>Confidence</t>
+    <t>Neutral</t>
   </si>
   <si>
     <t>I counted twenty punches here, all to the face, that's quite a beating, in Cobra Kai when Hawk gives the bully guy a legendary beating there's a total of fifteen hits to the face in that, so that bully got 75% of a fatal beating if you compare the numbers</t>
   </si>
   <si>
-    <t>Very Positive</t>
+    <t>Very Negative</t>
   </si>
   <si>
     <t>as a exjunkie i have one thing..the hole scene and series are amazing..BUT ON  AMPHETAMIN BEATING A GUY TO DEATH..and being able to eat.....hello that is what i call ...BOSS WHICH BECOMES ADDICTEF FROM COCAIEN OR TUCO ARE ALREDY DETH..miss th at part...to show all teen guys..like me....i was a fool....thinking being addicted make me special..is not..BUT AMZAZIN...and of course...RELAX..HE IS THEE BOSS OF MOB....not a CEO....HE CANT ALLOW TO SOMEBODY IN PUBLIC HUMILATE HIM..BUT ALREADY KNOW ..TUCO IS GONE...BUT TO FAT FOR A CRYSTAL USER..OR?</t>
   </si>
   <si>
-    <t>Neutral</t>
-  </si>
-  <si>
     <t>I wish they would of made a few more deals instead of just 3 lol</t>
   </si>
   <si>
-    <t>Very Negative</t>
-  </si>
-  <si>
     <t>Have met a few guys with tucos personality. They are very interesting individuals.</t>
+  </si>
+  <si>
+    <t>Positive</t>
   </si>
   <si>
     <t>Anyone else here bc @1minutetalkshow</t>
@@ -73,6 +64,9 @@
     <t>This is how my mom reacts when ppl tell her to relax.</t>
   </si>
   <si>
+    <t>Very Positive</t>
+  </si>
+  <si>
     <t>this was the moment Heisenberg became Walter White.</t>
   </si>
   <si>
@@ -109,6 +103,9 @@
   <si>
     <t>He almost got the:
  lets go waltuh  BOOM* shot on the back of the head</t>
+  </si>
+  <si>
+    <t>Negative</t>
   </si>
   <si>
     <t>That "Yeahh"
@@ -168,12 +165,6 @@
   </si>
   <si>
     <t>awesome.</t>
-  </si>
-  <si>
-    <t>Positive</t>
-  </si>
-  <si>
-    <t>Negative</t>
   </si>
 </sst>
 </file>
@@ -437,11 +428,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22 N22"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10 D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="46.140625" style="1" customWidth="1"/>
     <col min="2" max="25" width="8.7109375" style="1" customWidth="1"/>
@@ -454,484 +445,1091 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
+      <c r="C1" s="1">
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1">
         <v>0.3</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
         <v>0.26</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="1">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
         <v>0.75</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="1">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1">
         <v>0.78</v>
       </c>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5"/>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5"/>
+      <c r="M5"/>
+      <c r="N5"/>
+      <c r="O5"/>
+      <c r="P5"/>
+      <c r="Q5"/>
+      <c r="R5"/>
+      <c r="S5"/>
+      <c r="T5"/>
+      <c r="U5"/>
+      <c r="V5"/>
+      <c r="W5"/>
+      <c r="X5"/>
+      <c r="Y5"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="1">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
         <v>0.75</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7"/>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
         <v>0.77</v>
       </c>
-      <c r="E7"/>
-      <c r="F7"/>
-      <c r="G7"/>
-      <c r="H7"/>
-      <c r="I7"/>
-      <c r="J7"/>
-      <c r="K7"/>
-      <c r="L7"/>
-      <c r="M7"/>
-      <c r="N7"/>
-      <c r="O7"/>
-      <c r="P7"/>
-      <c r="Q7"/>
-      <c r="R7"/>
-      <c r="S7"/>
-      <c r="T7"/>
-      <c r="U7"/>
-      <c r="V7"/>
-      <c r="W7"/>
-      <c r="X7"/>
-      <c r="Y7"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="1">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1">
         <v>0.52</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="1">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="1">
         <v>0.54</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="1">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1">
         <v>0.64</v>
       </c>
     </row>
     <row r="11" spans="1:25" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11"/>
-      <c r="C11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1">
         <v>0.54</v>
       </c>
-      <c r="E11"/>
-      <c r="F11"/>
-      <c r="G11"/>
-      <c r="H11"/>
-      <c r="I11"/>
-      <c r="J11"/>
-      <c r="K11"/>
-      <c r="L11"/>
-      <c r="M11"/>
-      <c r="N11"/>
-      <c r="O11"/>
-      <c r="P11"/>
-      <c r="Q11"/>
-      <c r="R11"/>
-      <c r="S11"/>
-      <c r="T11"/>
-      <c r="U11"/>
-      <c r="V11"/>
-      <c r="W11"/>
-      <c r="X11"/>
-      <c r="Y11"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="1">
+        <v>15</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
         <v>0.94</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="1">
+        <v>16</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1">
         <v>0.79</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="1">
+        <v>17</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="1">
+        <v>18</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="1">
         <v>0.72</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="1">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="B18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="1">
-        <v>0.55000000000000004</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="C19" s="1">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="1">
-        <v>0.31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="B20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" s="1">
-        <v>0.57999999999999996</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" s="1">
-        <v>0.82</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="C21" s="1">
+        <v>0.41</v>
+      </c>
+      <c r="E21"/>
+      <c r="F21"/>
+      <c r="G21"/>
+      <c r="H21"/>
+      <c r="I21"/>
+      <c r="J21"/>
+      <c r="K21"/>
+      <c r="L21"/>
+      <c r="M21"/>
+      <c r="N21"/>
+      <c r="O21"/>
+      <c r="P21"/>
+      <c r="Q21"/>
+      <c r="R21"/>
+      <c r="S21"/>
+      <c r="T21"/>
+      <c r="U21"/>
+      <c r="V21"/>
+      <c r="W21"/>
+      <c r="X21"/>
+      <c r="Y21"/>
+    </row>
+    <row r="22" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D21" s="1">
-        <v>0.41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="B22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0.68</v>
+      </c>
+      <c r="E22"/>
+      <c r="F22"/>
+      <c r="G22"/>
+      <c r="H22"/>
+      <c r="I22"/>
+      <c r="J22"/>
+      <c r="K22"/>
+      <c r="L22"/>
+      <c r="M22"/>
+      <c r="N22"/>
+      <c r="O22"/>
+      <c r="P22"/>
+      <c r="Q22"/>
+      <c r="R22"/>
+      <c r="S22"/>
+      <c r="T22"/>
+      <c r="U22"/>
+      <c r="V22"/>
+      <c r="W22"/>
+      <c r="X22"/>
+      <c r="Y22"/>
+    </row>
+    <row r="23" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" s="1">
-        <v>0.68</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="B23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0.36</v>
+      </c>
+      <c r="E23"/>
+      <c r="F23"/>
+      <c r="G23"/>
+      <c r="H23"/>
+      <c r="I23"/>
+      <c r="J23"/>
+      <c r="K23"/>
+      <c r="L23"/>
+      <c r="M23"/>
+      <c r="N23"/>
+      <c r="O23"/>
+      <c r="P23"/>
+      <c r="Q23"/>
+      <c r="R23"/>
+      <c r="S23"/>
+      <c r="T23"/>
+      <c r="U23"/>
+      <c r="V23"/>
+      <c r="W23"/>
+      <c r="X23"/>
+      <c r="Y23"/>
+    </row>
+    <row r="24" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D23" s="1">
-        <v>0.36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="B24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0.74</v>
+      </c>
+      <c r="E24"/>
+      <c r="F24"/>
+      <c r="G24"/>
+      <c r="H24"/>
+      <c r="I24"/>
+      <c r="J24"/>
+      <c r="K24"/>
+      <c r="L24"/>
+      <c r="M24"/>
+      <c r="N24"/>
+      <c r="O24"/>
+      <c r="P24"/>
+      <c r="Q24"/>
+      <c r="R24"/>
+      <c r="S24"/>
+      <c r="T24"/>
+      <c r="U24"/>
+      <c r="V24"/>
+      <c r="W24"/>
+      <c r="X24"/>
+      <c r="Y24"/>
+    </row>
+    <row r="25" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="B25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0.38</v>
+      </c>
+      <c r="E25"/>
+      <c r="F25"/>
+      <c r="G25"/>
+      <c r="H25"/>
+      <c r="I25"/>
+      <c r="J25"/>
+      <c r="K25"/>
+      <c r="L25"/>
+      <c r="M25"/>
+      <c r="N25"/>
+      <c r="O25"/>
+      <c r="P25"/>
+      <c r="Q25"/>
+      <c r="R25"/>
+      <c r="S25"/>
+      <c r="T25"/>
+      <c r="U25"/>
+      <c r="V25"/>
+      <c r="W25"/>
+      <c r="X25"/>
+      <c r="Y25"/>
+    </row>
+    <row r="26" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D24" s="1">
-        <v>0.74</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D25" s="1">
-        <v>0.38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="C26" s="1">
+        <v>0.97</v>
+      </c>
+      <c r="E26"/>
+      <c r="F26"/>
+      <c r="G26"/>
+      <c r="H26"/>
+      <c r="I26"/>
+      <c r="J26"/>
+      <c r="K26"/>
+      <c r="L26"/>
+      <c r="M26"/>
+      <c r="N26"/>
+      <c r="O26"/>
+      <c r="P26"/>
+      <c r="Q26"/>
+      <c r="R26"/>
+      <c r="S26"/>
+      <c r="T26"/>
+      <c r="U26"/>
+      <c r="V26"/>
+      <c r="W26"/>
+      <c r="X26"/>
+      <c r="Y26"/>
+    </row>
+    <row r="27" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D26" s="1">
-        <v>0.97</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="B27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0.63</v>
+      </c>
+      <c r="E27"/>
+      <c r="F27"/>
+      <c r="G27"/>
+      <c r="H27"/>
+      <c r="I27"/>
+      <c r="J27"/>
+      <c r="K27"/>
+      <c r="L27"/>
+      <c r="M27"/>
+      <c r="N27"/>
+      <c r="O27"/>
+      <c r="P27"/>
+      <c r="Q27"/>
+      <c r="R27"/>
+      <c r="S27"/>
+      <c r="T27"/>
+      <c r="U27"/>
+      <c r="V27"/>
+      <c r="W27"/>
+      <c r="X27"/>
+      <c r="Y27"/>
+    </row>
+    <row r="28" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D27" s="1">
-        <v>0.63</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="B28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0.64</v>
+      </c>
+      <c r="E28"/>
+      <c r="F28"/>
+      <c r="G28"/>
+      <c r="H28"/>
+      <c r="I28"/>
+      <c r="J28"/>
+      <c r="K28"/>
+      <c r="L28"/>
+      <c r="M28"/>
+      <c r="N28"/>
+      <c r="O28"/>
+      <c r="P28"/>
+      <c r="Q28"/>
+      <c r="R28"/>
+      <c r="S28"/>
+      <c r="T28"/>
+      <c r="U28"/>
+      <c r="V28"/>
+      <c r="W28"/>
+      <c r="X28"/>
+      <c r="Y28"/>
+    </row>
+    <row r="29" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="B29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="E29"/>
+      <c r="F29"/>
+      <c r="G29"/>
+      <c r="H29"/>
+      <c r="I29"/>
+      <c r="J29"/>
+      <c r="K29"/>
+      <c r="L29"/>
+      <c r="M29"/>
+      <c r="N29"/>
+      <c r="O29"/>
+      <c r="P29"/>
+      <c r="Q29"/>
+      <c r="R29"/>
+      <c r="S29"/>
+      <c r="T29"/>
+      <c r="U29"/>
+      <c r="V29"/>
+      <c r="W29"/>
+      <c r="X29"/>
+      <c r="Y29"/>
+    </row>
+    <row r="30" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D28" s="1">
-        <v>0.64</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C29" s="1" t="s">
+      <c r="C30" s="1">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="E30"/>
+      <c r="F30"/>
+      <c r="G30"/>
+      <c r="H30"/>
+      <c r="I30"/>
+      <c r="J30"/>
+      <c r="K30"/>
+      <c r="L30"/>
+      <c r="M30"/>
+      <c r="N30"/>
+      <c r="O30"/>
+      <c r="P30"/>
+      <c r="Q30"/>
+      <c r="R30"/>
+      <c r="S30"/>
+      <c r="T30"/>
+      <c r="U30"/>
+      <c r="V30"/>
+      <c r="W30"/>
+      <c r="X30"/>
+      <c r="Y30"/>
+    </row>
+    <row r="31" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0.46</v>
+      </c>
+      <c r="E31"/>
+      <c r="F31"/>
+      <c r="G31"/>
+      <c r="H31"/>
+      <c r="I31"/>
+      <c r="J31"/>
+      <c r="K31"/>
+      <c r="L31"/>
+      <c r="M31"/>
+      <c r="N31"/>
+      <c r="O31"/>
+      <c r="P31"/>
+      <c r="Q31"/>
+      <c r="R31"/>
+      <c r="S31"/>
+      <c r="T31"/>
+      <c r="U31"/>
+      <c r="V31"/>
+      <c r="W31"/>
+      <c r="X31"/>
+      <c r="Y31"/>
+    </row>
+    <row r="32" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="E32"/>
+      <c r="F32"/>
+      <c r="G32"/>
+      <c r="H32"/>
+      <c r="I32"/>
+      <c r="J32"/>
+      <c r="K32"/>
+      <c r="L32"/>
+      <c r="M32"/>
+      <c r="N32"/>
+      <c r="O32"/>
+      <c r="P32"/>
+      <c r="Q32"/>
+      <c r="R32"/>
+      <c r="S32"/>
+      <c r="T32"/>
+      <c r="U32"/>
+      <c r="V32"/>
+      <c r="W32"/>
+      <c r="X32"/>
+      <c r="Y32"/>
+    </row>
+    <row r="33" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0.59</v>
+      </c>
+      <c r="E33"/>
+      <c r="F33"/>
+      <c r="G33"/>
+      <c r="H33"/>
+      <c r="I33"/>
+      <c r="J33"/>
+      <c r="K33"/>
+      <c r="L33"/>
+      <c r="M33"/>
+      <c r="N33"/>
+      <c r="O33"/>
+      <c r="P33"/>
+      <c r="Q33"/>
+      <c r="R33"/>
+      <c r="S33"/>
+      <c r="T33"/>
+      <c r="U33"/>
+      <c r="V33"/>
+      <c r="W33"/>
+      <c r="X33"/>
+      <c r="Y33"/>
+    </row>
+    <row r="34" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D29" s="1">
+      <c r="C34" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="E34"/>
+      <c r="F34"/>
+      <c r="G34"/>
+      <c r="H34"/>
+      <c r="I34"/>
+      <c r="J34"/>
+      <c r="K34"/>
+      <c r="L34"/>
+      <c r="M34"/>
+      <c r="N34"/>
+      <c r="O34"/>
+      <c r="P34"/>
+      <c r="Q34"/>
+      <c r="R34"/>
+      <c r="S34"/>
+      <c r="T34"/>
+      <c r="U34"/>
+      <c r="V34"/>
+      <c r="W34"/>
+      <c r="X34"/>
+      <c r="Y34"/>
+    </row>
+    <row r="35" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" s="1">
+        <v>0.61</v>
+      </c>
+      <c r="E35"/>
+      <c r="F35"/>
+      <c r="G35"/>
+      <c r="H35"/>
+      <c r="I35"/>
+      <c r="J35"/>
+      <c r="K35"/>
+      <c r="L35"/>
+      <c r="M35"/>
+      <c r="N35"/>
+      <c r="O35"/>
+      <c r="P35"/>
+      <c r="Q35"/>
+      <c r="R35"/>
+      <c r="S35"/>
+      <c r="T35"/>
+      <c r="U35"/>
+      <c r="V35"/>
+      <c r="W35"/>
+      <c r="X35"/>
+      <c r="Y35"/>
+    </row>
+    <row r="36" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" s="1">
+        <v>0.77</v>
+      </c>
+      <c r="E36"/>
+      <c r="F36"/>
+      <c r="G36"/>
+      <c r="H36"/>
+      <c r="I36"/>
+      <c r="J36"/>
+      <c r="K36"/>
+      <c r="L36"/>
+      <c r="M36"/>
+      <c r="N36"/>
+      <c r="O36"/>
+      <c r="P36"/>
+      <c r="Q36"/>
+      <c r="R36"/>
+      <c r="S36"/>
+      <c r="T36"/>
+      <c r="U36"/>
+      <c r="V36"/>
+      <c r="W36"/>
+      <c r="X36"/>
+      <c r="Y36"/>
+    </row>
+    <row r="37" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="1">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D30" s="1">
-        <v>0.56000000000000005</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D31" s="1">
-        <v>0.46</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D32" s="1">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D33" s="1">
-        <v>0.59</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D34" s="1">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D35" s="1">
-        <v>0.61</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D36" s="1">
-        <v>0.77</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="E37"/>
+      <c r="F37"/>
+      <c r="G37"/>
+      <c r="H37"/>
+      <c r="I37"/>
+      <c r="J37"/>
+      <c r="K37"/>
+      <c r="L37"/>
+      <c r="M37"/>
+      <c r="N37"/>
+      <c r="O37"/>
+      <c r="P37"/>
+      <c r="Q37"/>
+      <c r="R37"/>
+      <c r="S37"/>
+      <c r="T37"/>
+      <c r="U37"/>
+      <c r="V37"/>
+      <c r="W37"/>
+      <c r="X37"/>
+      <c r="Y37"/>
+    </row>
+    <row r="38" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D37" s="1">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="B38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" s="1">
+        <v>0.42</v>
+      </c>
+      <c r="E38"/>
+      <c r="F38"/>
+      <c r="G38"/>
+      <c r="H38"/>
+      <c r="I38"/>
+      <c r="J38"/>
+      <c r="K38"/>
+      <c r="L38"/>
+      <c r="M38"/>
+      <c r="N38"/>
+      <c r="O38"/>
+      <c r="P38"/>
+      <c r="Q38"/>
+      <c r="R38"/>
+      <c r="S38"/>
+      <c r="T38"/>
+      <c r="U38"/>
+      <c r="V38"/>
+      <c r="W38"/>
+      <c r="X38"/>
+      <c r="Y38"/>
+    </row>
+    <row r="39" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D38" s="1">
-        <v>0.42</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D39" s="1">
+      <c r="B39" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="C39" s="1">
+        <v>1</v>
+      </c>
+      <c r="E39"/>
+      <c r="F39"/>
+      <c r="G39"/>
+      <c r="H39"/>
+      <c r="I39"/>
+      <c r="J39"/>
+      <c r="K39"/>
+      <c r="L39"/>
+      <c r="M39"/>
+      <c r="N39"/>
+      <c r="O39"/>
+      <c r="P39"/>
+      <c r="Q39"/>
+      <c r="R39"/>
+      <c r="S39"/>
+      <c r="T39"/>
+      <c r="U39"/>
+      <c r="V39"/>
+      <c r="W39"/>
+      <c r="X39"/>
+      <c r="Y39"/>
+    </row>
+    <row r="40" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40"/>
+      <c r="B40"/>
+      <c r="C40"/>
+      <c r="D40"/>
+      <c r="E40"/>
+      <c r="F40"/>
+      <c r="G40"/>
+      <c r="H40"/>
+      <c r="I40"/>
+      <c r="J40"/>
+      <c r="K40"/>
+      <c r="L40"/>
+      <c r="M40"/>
+      <c r="N40"/>
+      <c r="O40"/>
+      <c r="P40"/>
+      <c r="Q40"/>
+      <c r="R40"/>
+      <c r="S40"/>
+      <c r="T40"/>
+      <c r="U40"/>
+      <c r="V40"/>
+      <c r="W40"/>
+      <c r="X40"/>
+      <c r="Y40"/>
+    </row>
+    <row r="41" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41"/>
+      <c r="B41"/>
+      <c r="C41"/>
+      <c r="D41"/>
+      <c r="E41"/>
+      <c r="F41"/>
+      <c r="G41"/>
+      <c r="H41"/>
+      <c r="I41"/>
+      <c r="J41"/>
+      <c r="K41"/>
+      <c r="L41"/>
+      <c r="M41"/>
+      <c r="N41"/>
+      <c r="O41"/>
+      <c r="P41"/>
+      <c r="Q41"/>
+      <c r="R41"/>
+      <c r="S41"/>
+      <c r="T41"/>
+      <c r="U41"/>
+      <c r="V41"/>
+      <c r="W41"/>
+      <c r="X41"/>
+      <c r="Y41"/>
+    </row>
+    <row r="42" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42"/>
+      <c r="B42"/>
+      <c r="C42"/>
+      <c r="D42"/>
+      <c r="E42"/>
+      <c r="F42"/>
+      <c r="G42"/>
+      <c r="H42"/>
+      <c r="I42"/>
+      <c r="J42"/>
+      <c r="K42"/>
+      <c r="L42"/>
+      <c r="M42"/>
+      <c r="N42"/>
+      <c r="O42"/>
+      <c r="P42"/>
+      <c r="Q42"/>
+      <c r="R42"/>
+      <c r="S42"/>
+      <c r="T42"/>
+      <c r="U42"/>
+      <c r="V42"/>
+      <c r="W42"/>
+      <c r="X42"/>
+      <c r="Y42"/>
+    </row>
+    <row r="43" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43"/>
+      <c r="B43"/>
+      <c r="C43"/>
+      <c r="D43"/>
+      <c r="E43"/>
+      <c r="F43"/>
+      <c r="G43"/>
+      <c r="H43"/>
+      <c r="I43"/>
+      <c r="J43"/>
+      <c r="K43"/>
+      <c r="L43"/>
+      <c r="M43"/>
+      <c r="N43"/>
+      <c r="O43"/>
+      <c r="P43"/>
+      <c r="Q43"/>
+      <c r="R43"/>
+      <c r="S43"/>
+      <c r="T43"/>
+      <c r="U43"/>
+      <c r="V43"/>
+      <c r="W43"/>
+      <c r="X43"/>
+      <c r="Y43"/>
+    </row>
+    <row r="44" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44"/>
+      <c r="B44"/>
+      <c r="C44"/>
+      <c r="D44"/>
+      <c r="E44"/>
+      <c r="F44"/>
+      <c r="G44"/>
+      <c r="H44"/>
+      <c r="I44"/>
+      <c r="J44"/>
+      <c r="K44"/>
+      <c r="L44"/>
+      <c r="M44"/>
+      <c r="N44"/>
+      <c r="O44"/>
+      <c r="P44"/>
+      <c r="Q44"/>
+      <c r="R44"/>
+      <c r="S44"/>
+      <c r="T44"/>
+      <c r="U44"/>
+      <c r="V44"/>
+      <c r="W44"/>
+      <c r="X44"/>
+      <c r="Y44"/>
+    </row>
+    <row r="45" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45"/>
+      <c r="B45"/>
+      <c r="C45"/>
+      <c r="D45"/>
+      <c r="E45"/>
+      <c r="F45"/>
+      <c r="G45"/>
+      <c r="H45"/>
+      <c r="I45"/>
+      <c r="J45"/>
+      <c r="K45"/>
+      <c r="L45"/>
+      <c r="M45"/>
+      <c r="N45"/>
+      <c r="O45"/>
+      <c r="P45"/>
+      <c r="Q45"/>
+      <c r="R45"/>
+      <c r="S45"/>
+      <c r="T45"/>
+      <c r="U45"/>
+      <c r="V45"/>
+      <c r="W45"/>
+      <c r="X45"/>
+      <c r="Y45"/>
+    </row>
+    <row r="46" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46"/>
+      <c r="B46"/>
+      <c r="C46"/>
+      <c r="D46"/>
+      <c r="E46"/>
+      <c r="F46"/>
+      <c r="G46"/>
+      <c r="H46"/>
+      <c r="I46"/>
+      <c r="J46"/>
+      <c r="K46"/>
+      <c r="L46"/>
+      <c r="M46"/>
+      <c r="N46"/>
+      <c r="O46"/>
+      <c r="P46"/>
+      <c r="Q46"/>
+      <c r="R46"/>
+      <c r="S46"/>
+      <c r="T46"/>
+      <c r="U46"/>
+      <c r="V46"/>
+      <c r="W46"/>
+      <c r="X46"/>
+      <c r="Y46"/>
+    </row>
+    <row r="47" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47"/>
+      <c r="B47"/>
+      <c r="C47"/>
+      <c r="D47"/>
+      <c r="E47"/>
+      <c r="F47"/>
+      <c r="G47"/>
+      <c r="H47"/>
+      <c r="I47"/>
+      <c r="J47"/>
+      <c r="K47"/>
+      <c r="L47"/>
+      <c r="M47"/>
+      <c r="N47"/>
+      <c r="O47"/>
+      <c r="P47"/>
+      <c r="Q47"/>
+      <c r="R47"/>
+      <c r="S47"/>
+      <c r="T47"/>
+      <c r="U47"/>
+      <c r="V47"/>
+      <c r="W47"/>
+      <c r="X47"/>
+      <c r="Y47"/>
+    </row>
+    <row r="48" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48"/>
+      <c r="B48"/>
+      <c r="C48"/>
+      <c r="D48"/>
+      <c r="E48"/>
+      <c r="F48"/>
+      <c r="G48"/>
+      <c r="H48"/>
+      <c r="I48"/>
+      <c r="J48"/>
+      <c r="K48"/>
+      <c r="L48"/>
+      <c r="M48"/>
+      <c r="N48"/>
+      <c r="O48"/>
+      <c r="P48"/>
+      <c r="Q48"/>
+      <c r="R48"/>
+      <c r="S48"/>
+      <c r="T48"/>
+      <c r="U48"/>
+      <c r="V48"/>
+      <c r="W48"/>
+      <c r="X48"/>
+      <c r="Y48"/>
+    </row>
     <row r="49" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="50" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add error handling for sentiment analysis
Co-Authored-By: Jia Tee <73531134+JJTee@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/SocialMediaAnalysis/Output/inputData.xlsx
+++ b/SocialMediaAnalysis/Output/inputData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoa-my.sharepoint.com/personal/xzha897_uoa_auckland_ac_nz/Documents/Documents/GitHub/social-media-analysis/SocialMediaAnalysis/Output/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xzha897\Documents\GitHub\social-media-analysis\SocialMediaAnalysis\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_88D8E44A8506AE2F867E1EB6D3D5462CEE13370C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BBF98293-5BFE-4874-8821-DFDD4141BF76}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A6FC290-6C6E-4FED-871C-5CB30949E1C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="1965" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>

</xml_diff>

<commit_message>
resolve conflicts with merge
Co-Authored-By: Jia Tee <73531134+JJTee@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/SocialMediaAnalysis/Output/inputData.xlsx
+++ b/SocialMediaAnalysis/Output/inputData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xzha897\Documents\GitHub\social-media-analysis\SocialMediaAnalysis\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A6FC290-6C6E-4FED-871C-5CB30949E1C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDFB9E75-11C8-4497-A43F-2398CB7B6481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="1965" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -20,18 +20,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
-    <t>very good comment</t>
+    <t>i hate this product</t>
   </si>
   <si>
-    <t>sigh not good</t>
+    <t xml:space="preserve"> this product is so fantastic its great</t>
   </si>
   <si>
-    <t>Positive</t>
+    <t xml:space="preserve"> i will never use this product again</t>
   </si>
   <si>
-    <t>Negative</t>
+    <t>Very Negative</t>
+  </si>
+  <si>
+    <t>Very Positive</t>
   </si>
 </sst>
 </file>
@@ -370,7 +373,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -381,10 +384,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C1">
-        <v>0.99</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -392,10 +395,21 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C2">
-        <v>0.66</v>
+      <c r="C3">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add logging to files
Co-Authored-By: Jia Tee <73531134+JJTee@users.noreply.github.com>
Co-Authored-By: wnoome <119922795+wnoome@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/SocialMediaAnalysis/Output/inputData.xlsx
+++ b/SocialMediaAnalysis/Output/inputData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xzha897\Documents\GitHub\social-media-analysis\SocialMediaAnalysis\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDFB9E75-11C8-4497-A43F-2398CB7B6481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83857D8-0BB1-48B4-9EED-7D899A44B1A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,21 +20,96 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
-  <si>
-    <t>i hate this product</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> this product is so fantastic its great</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> i will never use this product again</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="30">
+  <si>
+    <t>Gus's last words were HAUWWWW</t>
+  </si>
+  <si>
+    <t>Mike's last words are perfect for him. That's the only part of his death that made sense, aside from how he should have saved Kailey.</t>
+  </si>
+  <si>
+    <t>Todd shouldn’t have tried to convert Walt into Catholicism, then Jesse wouldn’t have killed him</t>
+  </si>
+  <si>
+    <t>Actually Gus’ last words would be HAAAAA</t>
+  </si>
+  <si>
+    <t>Mike's go the hardest no doubt</t>
+  </si>
+  <si>
+    <t>You forgot:</t>
+  </si>
+  <si>
+    <t>Emilio, Lydia and Jane most likely had different last words than what we see on screen. All we’re alive for hours after their final in-show lines.</t>
+  </si>
+  <si>
+    <t>Gus’ last words are so ironic if you think about it</t>
+  </si>
+  <si>
+    <t>This was really interesting. It’s hard to create/find fresh content for this subreddit anymore. You did it. Props</t>
+  </si>
+  <si>
+    <t>Walt’s real last words were said in that look he gave to Jesse in the finale.</t>
+  </si>
+  <si>
+    <t>Drew Sharp: damn this tarantula looking really sick!</t>
+  </si>
+  <si>
+    <t>Wasnt juans last word what is that? Could be misunderstanding que se so tho</t>
+  </si>
+  <si>
+    <t>Wasn't Combo's last word "Bounce?"</t>
+  </si>
+  <si>
+    <t>Ding ding ding ding - Hector</t>
+  </si>
+  <si>
+    <t>Combos are wrong his were.. “what I say? get out of here.. go”</t>
+  </si>
+  <si>
+    <t>I want my last words to be "I am breaking bad" as I cause the Earth to implode</t>
+  </si>
+  <si>
+    <t>Marie..."well what do you think? so I was shopping the other day and the assistant says to me do you know I fancy a drink let's have a margherita so she says anyway how's Walt? I've been thinking and maybe we should have a big get together for Holly's birthday you know it's only once a year so we need a big get together ooh is that new wallpaper? so I was working the other day and blah blah blah blah you know?"</t>
+  </si>
+  <si>
+    <t>Random guy in the parking lot: Jesus!</t>
+  </si>
+  <si>
+    <t>All shit except for hank.</t>
+  </si>
+  <si>
+    <t>Todd shouldnâ€™t have tried to convert Walt into Catholicism, then Jesse wouldnâ€™t have killed him</t>
+  </si>
+  <si>
+    <t>Actually Gusâ€™ last words would be HAAAAA</t>
+  </si>
+  <si>
+    <t>Emilio, Lydia and Jane most likely had different last words than what we see on screen. All weâ€™re alive for hours after their final in-show lines.</t>
+  </si>
+  <si>
+    <t>Gusâ€™ last words are so ironic if you think about it</t>
+  </si>
+  <si>
+    <t>This was really interesting. Itâ€™s hard to create/find fresh content for this subreddit anymore. You did it. Props</t>
+  </si>
+  <si>
+    <t>Waltâ€™s real last words were said in that look he gave to Jesse in the finale.</t>
+  </si>
+  <si>
+    <t>Combos are wrong his were.. â€œwhat I say? get out of here.. goâ€</t>
+  </si>
+  <si>
+    <t>Neutral</t>
+  </si>
+  <si>
+    <t>Positive</t>
+  </si>
+  <si>
+    <t>Negative</t>
   </si>
   <si>
     <t>Very Negative</t>
-  </si>
-  <si>
-    <t>Very Positive</t>
   </si>
 </sst>
 </file>
@@ -373,9 +448,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -384,10 +459,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C1">
-        <v>1</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -395,10 +470,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="C2">
-        <v>0.98</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -406,10 +481,1022 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="C3">
-        <v>0.5</v>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" t="s">
+        <v>27</v>
+      </c>
+      <c r="C36">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37" t="s">
+        <v>28</v>
+      </c>
+      <c r="C37">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38" t="s">
+        <v>26</v>
+      </c>
+      <c r="C38">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" t="s">
+        <v>26</v>
+      </c>
+      <c r="C39">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" t="s">
+        <v>27</v>
+      </c>
+      <c r="C40">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" t="s">
+        <v>26</v>
+      </c>
+      <c r="C41">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>20</v>
+      </c>
+      <c r="B42" t="s">
+        <v>28</v>
+      </c>
+      <c r="C42">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" t="s">
+        <v>26</v>
+      </c>
+      <c r="C43">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44" t="s">
+        <v>26</v>
+      </c>
+      <c r="C44">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>21</v>
+      </c>
+      <c r="B45" t="s">
+        <v>27</v>
+      </c>
+      <c r="C45">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>22</v>
+      </c>
+      <c r="B46" t="s">
+        <v>26</v>
+      </c>
+      <c r="C46">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>23</v>
+      </c>
+      <c r="B47" t="s">
+        <v>26</v>
+      </c>
+      <c r="C47">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>24</v>
+      </c>
+      <c r="B48" t="s">
+        <v>26</v>
+      </c>
+      <c r="C48">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>10</v>
+      </c>
+      <c r="B49" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>11</v>
+      </c>
+      <c r="B50" t="s">
+        <v>26</v>
+      </c>
+      <c r="C50">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>12</v>
+      </c>
+      <c r="B51" t="s">
+        <v>26</v>
+      </c>
+      <c r="C51">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>13</v>
+      </c>
+      <c r="B52" t="s">
+        <v>26</v>
+      </c>
+      <c r="C52">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>25</v>
+      </c>
+      <c r="B53" t="s">
+        <v>29</v>
+      </c>
+      <c r="C53">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>15</v>
+      </c>
+      <c r="B54" t="s">
+        <v>29</v>
+      </c>
+      <c r="C54">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>16</v>
+      </c>
+      <c r="B55" t="s">
+        <v>27</v>
+      </c>
+      <c r="C55">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>17</v>
+      </c>
+      <c r="B56" t="s">
+        <v>28</v>
+      </c>
+      <c r="C56">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>18</v>
+      </c>
+      <c r="B57" t="s">
+        <v>26</v>
+      </c>
+      <c r="C57">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>0</v>
+      </c>
+      <c r="B58" t="s">
+        <v>26</v>
+      </c>
+      <c r="C58">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>1</v>
+      </c>
+      <c r="B59" t="s">
+        <v>27</v>
+      </c>
+      <c r="C59">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>19</v>
+      </c>
+      <c r="B60" t="s">
+        <v>26</v>
+      </c>
+      <c r="C60">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>20</v>
+      </c>
+      <c r="B61" t="s">
+        <v>28</v>
+      </c>
+      <c r="C61">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>4</v>
+      </c>
+      <c r="B62" t="s">
+        <v>26</v>
+      </c>
+      <c r="C62">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>5</v>
+      </c>
+      <c r="B63" t="s">
+        <v>26</v>
+      </c>
+      <c r="C63">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>21</v>
+      </c>
+      <c r="B64" t="s">
+        <v>27</v>
+      </c>
+      <c r="C64">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>22</v>
+      </c>
+      <c r="B65" t="s">
+        <v>26</v>
+      </c>
+      <c r="C65">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>23</v>
+      </c>
+      <c r="B66" t="s">
+        <v>26</v>
+      </c>
+      <c r="C66">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>24</v>
+      </c>
+      <c r="B67" t="s">
+        <v>26</v>
+      </c>
+      <c r="C67">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>10</v>
+      </c>
+      <c r="B68" t="s">
+        <v>26</v>
+      </c>
+      <c r="C68">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>11</v>
+      </c>
+      <c r="B69" t="s">
+        <v>26</v>
+      </c>
+      <c r="C69">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>12</v>
+      </c>
+      <c r="B70" t="s">
+        <v>26</v>
+      </c>
+      <c r="C70">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>13</v>
+      </c>
+      <c r="B71" t="s">
+        <v>26</v>
+      </c>
+      <c r="C71">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>25</v>
+      </c>
+      <c r="B72" t="s">
+        <v>29</v>
+      </c>
+      <c r="C72">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>15</v>
+      </c>
+      <c r="B73" t="s">
+        <v>29</v>
+      </c>
+      <c r="C73">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>16</v>
+      </c>
+      <c r="B74" t="s">
+        <v>27</v>
+      </c>
+      <c r="C74">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>17</v>
+      </c>
+      <c r="B75" t="s">
+        <v>28</v>
+      </c>
+      <c r="C75">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>18</v>
+      </c>
+      <c r="B76" t="s">
+        <v>26</v>
+      </c>
+      <c r="C76">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>0</v>
+      </c>
+      <c r="B77" t="s">
+        <v>26</v>
+      </c>
+      <c r="C77">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>1</v>
+      </c>
+      <c r="B78" t="s">
+        <v>27</v>
+      </c>
+      <c r="C78">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>19</v>
+      </c>
+      <c r="B79" t="s">
+        <v>26</v>
+      </c>
+      <c r="C79">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>20</v>
+      </c>
+      <c r="B80" t="s">
+        <v>28</v>
+      </c>
+      <c r="C80">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>4</v>
+      </c>
+      <c r="B81" t="s">
+        <v>26</v>
+      </c>
+      <c r="C81">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>5</v>
+      </c>
+      <c r="B82" t="s">
+        <v>26</v>
+      </c>
+      <c r="C82">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>21</v>
+      </c>
+      <c r="B83" t="s">
+        <v>27</v>
+      </c>
+      <c r="C83">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>22</v>
+      </c>
+      <c r="B84" t="s">
+        <v>26</v>
+      </c>
+      <c r="C84">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>23</v>
+      </c>
+      <c r="B85" t="s">
+        <v>26</v>
+      </c>
+      <c r="C85">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>24</v>
+      </c>
+      <c r="B86" t="s">
+        <v>26</v>
+      </c>
+      <c r="C86">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>10</v>
+      </c>
+      <c r="B87" t="s">
+        <v>26</v>
+      </c>
+      <c r="C87">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>11</v>
+      </c>
+      <c r="B88" t="s">
+        <v>26</v>
+      </c>
+      <c r="C88">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>12</v>
+      </c>
+      <c r="B89" t="s">
+        <v>26</v>
+      </c>
+      <c r="C89">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>13</v>
+      </c>
+      <c r="B90" t="s">
+        <v>26</v>
+      </c>
+      <c r="C90">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>25</v>
+      </c>
+      <c r="B91" t="s">
+        <v>29</v>
+      </c>
+      <c r="C91">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>15</v>
+      </c>
+      <c r="B92" t="s">
+        <v>29</v>
+      </c>
+      <c r="C92">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>16</v>
+      </c>
+      <c r="B93" t="s">
+        <v>27</v>
+      </c>
+      <c r="C93">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>17</v>
+      </c>
+      <c r="B94" t="s">
+        <v>28</v>
+      </c>
+      <c r="C94">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>18</v>
+      </c>
+      <c r="B95" t="s">
+        <v>26</v>
+      </c>
+      <c r="C95">
+        <v>0.92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reddit: Use proper UiPath selectors for more robust comment retrieval
We use properly constructed manual selectors as to retrieve data
regardless of the source page.
</commit_message>
<xml_diff>
--- a/SocialMediaAnalysis/Output/inputData.xlsx
+++ b/SocialMediaAnalysis/Output/inputData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xzha897\Documents\GitHub\social-media-analysis\SocialMediaAnalysis\Output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjak923\Documents\social-media-analysis\SocialMediaAnalysis\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A1EFDC-D076-42F0-A808-660BF9CD4C6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD0E01B5-EFF5-490A-AE62-6EF40F2EB25D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -20,84 +20,402 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="30">
-  <si>
-    <t>Gus's last words were HAUWWWW</t>
-  </si>
-  <si>
-    <t>Mike's last words are perfect for him. That's the only part of his death that made sense, aside from how he should have saved Kailey.</t>
-  </si>
-  <si>
-    <t>Todd shouldn’t have tried to convert Walt into Catholicism, then Jesse wouldn’t have killed him</t>
-  </si>
-  <si>
-    <t>Actually Gus’ last words would be HAAAAA</t>
-  </si>
-  <si>
-    <t>Mike's go the hardest no doubt</t>
-  </si>
-  <si>
-    <t>You forgot:</t>
-  </si>
-  <si>
-    <t>Emilio, Lydia and Jane most likely had different last words than what we see on screen. All we’re alive for hours after their final in-show lines.</t>
-  </si>
-  <si>
-    <t>Gus’ last words are so ironic if you think about it</t>
-  </si>
-  <si>
-    <t>This was really interesting. It’s hard to create/find fresh content for this subreddit anymore. You did it. Props</t>
-  </si>
-  <si>
-    <t>Walt’s real last words were said in that look he gave to Jesse in the finale.</t>
-  </si>
-  <si>
-    <t>Drew Sharp: damn this tarantula looking really sick!</t>
-  </si>
-  <si>
-    <t>Wasnt juans last word what is that? Could be misunderstanding que se so tho</t>
-  </si>
-  <si>
-    <t>Wasn't Combo's last word "Bounce?"</t>
-  </si>
-  <si>
-    <t>Ding ding ding ding - Hector</t>
-  </si>
-  <si>
-    <t>Combos are wrong his were.. “what I say? get out of here.. go”</t>
-  </si>
-  <si>
-    <t>I want my last words to be "I am breaking bad" as I cause the Earth to implode</t>
-  </si>
-  <si>
-    <t>Marie..."well what do you think? so I was shopping the other day and the assistant says to me do you know I fancy a drink let's have a margherita so she says anyway how's Walt? I've been thinking and maybe we should have a big get together for Holly's birthday you know it's only once a year so we need a big get together ooh is that new wallpaper? so I was working the other day and blah blah blah blah you know?"</t>
-  </si>
-  <si>
-    <t>Random guy in the parking lot: Jesus!</t>
-  </si>
-  <si>
-    <t>All shit except for hank.</t>
-  </si>
-  <si>
-    <t>Todd shouldnâ€™t have tried to convert Walt into Catholicism, then Jesse wouldnâ€™t have killed him</t>
-  </si>
-  <si>
-    <t>Actually Gusâ€™ last words would be HAAAAA</t>
-  </si>
-  <si>
-    <t>Emilio, Lydia and Jane most likely had different last words than what we see on screen. All weâ€™re alive for hours after their final in-show lines.</t>
-  </si>
-  <si>
-    <t>Gusâ€™ last words are so ironic if you think about it</t>
-  </si>
-  <si>
-    <t>This was really interesting. Itâ€™s hard to create/find fresh content for this subreddit anymore. You did it. Props</t>
-  </si>
-  <si>
-    <t>Waltâ€™s real last words were said in that look he gave to Jesse in the finale.</t>
-  </si>
-  <si>
-    <t>Combos are wrong his were.. â€œwhat I say? get out of here.. goâ€</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="125">
+  <si>
+    <t>I am laughing way too hard at this.
+Just picturing him coming and going jump scaring by yelling Snips at her from around corners.</t>
+  </si>
+  <si>
+    <t>The show becomes a Paranoia thriller for Ahsoka</t>
+  </si>
+  <si>
+    <t>I honestly kinda like the idea.</t>
+  </si>
+  <si>
+    <t>Tbh, its what I wanted the obi-wan show to be</t>
+  </si>
+  <si>
+    <t>Anakin jump scares!</t>
+  </si>
+  <si>
+    <t>This is where the fun begins XD.
+Seriously though, Obi Wan yelling at the air could start the crazy Ben rumors that Luke talks about in A New Hope.</t>
+  </si>
+  <si>
+    <t>"I said Cato Neimoidia doesn't count!"
+"There's Old Ben again."</t>
+  </si>
+  <si>
+    <t>Tuskens: (These settlers are getting worse all the time!)</t>
+  </si>
+  <si>
+    <t>If you watch the Not Obi-wan channel on YouTube, it’s Obi, force ghost Qui-gonn, and Anakin watching Star Wars stuff</t>
+  </si>
+  <si>
+    <t>Such a good channel</t>
+  </si>
+  <si>
+    <t>One of my favorite channels is "The Farce Awakens"! They have parodies of the sequel trilogy characters, including Rey, Finn, Poe, Leia, Ben/Kylo, Han, Luke, Hux, and Phasma.</t>
+  </si>
+  <si>
+    <t>This is exactly what I predicted/wanted too. I don’t hate what they did, but I wish we got more PTSD Obi-Wan memories/visions/nightmares vs full on adventure.</t>
+  </si>
+  <si>
+    <t>Completely agree. If Obi-Wan got the Samurai Jack Season 5 treatment, we would have a better show overall</t>
+  </si>
+  <si>
+    <t>If Disney wasn’t the owner of Star Wars we would’ve gotten a better show overall…</t>
+  </si>
+  <si>
+    <t>It would’ve been good if people gave Solo a chance. Kenobi was a movie originally but because people didn’t give Solo a chance without Ford despite it being a decent movie, they decided to scrap the movie idea</t>
+  </si>
+  <si>
+    <t>That show was bafflingly mishandled.</t>
+  </si>
+  <si>
+    <t>Force Ghost Qui-Gon, aka "The Phantom Menace"</t>
+  </si>
+  <si>
+    <t>but Vader hadn't died yet</t>
+  </si>
+  <si>
+    <t>I’m still mad you lied to get on the Citadel mission Snips. Don’t make me get Plo’s ghost and talk it out</t>
+  </si>
+  <si>
+    <t>I can imagine him being petty by knocking stuff off shelves with the force</t>
+  </si>
+  <si>
+    <t>Catakin Shelfwalker</t>
+  </si>
+  <si>
+    <t>Ahsoka: ANAKIN NO!
+The Chosen One: I am inevitable knocks over item</t>
+  </si>
+  <si>
+    <t>That cup. That cup is the chosen one.</t>
+  </si>
+  <si>
+    <t>The force is a pathway to many abilities considered to be unnatural</t>
+  </si>
+  <si>
+    <t>takes out a spray bottle and squirts water at Anakin</t>
+  </si>
+  <si>
+    <t>sand would work better</t>
+  </si>
+  <si>
+    <t>Pocket sand!</t>
+  </si>
+  <si>
+    <t>Captain howdy actually</t>
+  </si>
+  <si>
+    <t>I would give a lot to see Plo’s ghost. Except he didn’t die. #PloEscapedAtTheLastMinute</t>
+  </si>
+  <si>
+    <t>I'm still impressed at Filoni's restraint. He didn't add a plot to have Plo learn Force Ghostification from Qui-gon or something.</t>
+  </si>
+  <si>
+    <t>“Is that what this is about?”</t>
+  </si>
+  <si>
+    <t>I was hoping Episode 9 would be Force Ghost Luke haunting Kylo while Kylo goes about his day. "What you doing there, sport? Putting your helmet back together? Good for you, kid"</t>
+  </si>
+  <si>
+    <t>"You're my nephew but you'll always be a little shit Ben."</t>
+  </si>
+  <si>
+    <t>I would've been happy with what the novelization did, which was essentially Force Ghost Luke haunting Leia, poking at her, teasing her.
+In the book, she knew that her time was approaching, and Luke was goading her into stubbornly refusing to let go until she reignited the light in her son. It was fun and sweet.</t>
+  </si>
+  <si>
+    <t>Honestly I would have watched it. Ghost Anakin just...Being around, but only in Ashoka's PoV scenes would have been a good build up to their final scene together as well.</t>
+  </si>
+  <si>
+    <t>Sabine thinking she's losing her sanity half the time would be hilarious</t>
+  </si>
+  <si>
+    <t>No new footage though. Just him smiling the way he did on Endor</t>
+  </si>
+  <si>
+    <t>If they leaned into it really hard then yeah. Just scenes of Ahsoka doing normal day-to-day things and Anakins ghost just standing next to her the whole time making passive aggressive comments the whole time. I’d watch that</t>
+  </si>
+  <si>
+    <t>Baylon kicking her butt. Anakin: goodness, Snips, have you learned nothing???</t>
+  </si>
+  <si>
+    <t>That but dialed up to 11. Anakin has taken on the mannerisms of Micheal Scott</t>
+  </si>
+  <si>
+    <t>I'm getting serious robot chicken "force ghost jar jar" vibes</t>
+  </si>
+  <si>
+    <t>Just watch that guy doing deepfakes of Anakin and Obi-wan reacting to Ahsoka thats basically what it is</t>
+  </si>
+  <si>
+    <t>and qui gon</t>
+  </si>
+  <si>
+    <t>Of course cannot forget that hungry ghost boy</t>
+  </si>
+  <si>
+    <t>lmao yeah, also I watched one of the episodes of them reacting and obiwan had to drug qui to not let him see anakin being vader ??</t>
+  </si>
+  <si>
+    <t>Classic I could watch them go for hours (and have) it's just fun</t>
+  </si>
+  <si>
+    <t>They should make an Anakin series with more clone wars adventures</t>
+  </si>
+  <si>
+    <t>3 years of war and 365 days in a year, we can definitely cram in some extra stories</t>
+  </si>
+  <si>
+    <t>I always feel like it is implied to take longer on screen than what the books state.</t>
+  </si>
+  <si>
+    <t>Just like breaking plates, turning lights on and off, and opening cupboards. But he’s still fully visible with a blue glow so he just looks like an asshole.</t>
+  </si>
+  <si>
+    <t>Anakin: Yeah, I run this shindig now Snips</t>
+  </si>
+  <si>
+    <t>Everyone around reacts with growing fear and dread about the ghost that haunts her and meanwhile she's just staring affectionately at his giggling blue-glowing form as he has the most fun he can with it</t>
+  </si>
+  <si>
+    <t>I'd watch it. The Ahsoka/Anakin interaction was, in my opinion, absolutely excellent. I think it spoke to Ahsoka's guilt that she abandoned Anakin when she left the Jedi order, and I'd love to see an arc where Ahsoka wrestles with those feelings and what I'm sure are years of questioning what would have happened if she had stayed with Anakin, and if their Jedi/padawan bond might have kept him from becoming Vader.</t>
+  </si>
+  <si>
+    <t>Like the little league coach whose son is the pitcher. "Come on, Snips! HUSTLE!"</t>
+  </si>
+  <si>
+    <t>Like the little league
+Coach whose son is the pitcher.
+"Come on, Snips! HUSTLE!"
+- ibepunkinmugs
+I detect haikus. And sometimes, successfully. Learn more about me.
+Opt out of replies: "haikusbot opt out" | Delete my comment: "haikusbot delete"</t>
+  </si>
+  <si>
+    <t>My theory is that Filioni keeps connecting the dots and Anakin also starts popping in on Luke and teasing him, so much so that he cut himself off from the force. “Gosh dad, I KNOW FORM 3” - Luke “Incorrect” - Force Ghost Anakin</t>
+  </si>
+  <si>
+    <t>Anakin: I'm the Chosen One, I'll be here past your death kiddo</t>
+  </si>
+  <si>
+    <t>I’m hoping Ahsoka and Sabine get back to their galaxy by Anakin guiding them through the world between worlds and they just pop out and land on Luke having breakfast. “Damn it Dad not again!”</t>
+  </si>
+  <si>
+    <t>Anakin: Get your scrawny ass up and go help stop Thrawn</t>
+  </si>
+  <si>
+    <t>"OOHoohOOHooh Snips the pear is floating all by itself oohOOHooh"
+"I can see you Master, also we can both actually levitate things"
+"And now the lights are flickering on and off ominously OOHoohOOH"</t>
+  </si>
+  <si>
+    <t>"I'm most certainly grumpy about this." -Old Obi-Wan</t>
+  </si>
+  <si>
+    <t>Ask I can think of right now is Ghost Nappa from DBZ Abridged.</t>
+  </si>
+  <si>
+    <t>Anakin: She took the space map
+Ahsoka:FUUUUUUUUUUUUUUUUUUUUUU-</t>
+  </si>
+  <si>
+    <t>Just imagine if their were hundreds of stormtroopers charging at her and she looked over her shoulder to see Anakin and asked him "master Skywalker there are too many of them what are we going to do!"</t>
+  </si>
+  <si>
+    <t>Anakin: That evil Vader smile he did in Obi-Wan Kenobi</t>
+  </si>
+  <si>
+    <t>“Anakin, go away, I need privacy to go to the bathroom.”
+“Incorrect.”</t>
+  </si>
+  <si>
+    <t>She must learn to defend herself while using the toilet, Form 8: The Sitting Style.</t>
+  </si>
+  <si>
+    <t>And Form 9: The Shitting Style</t>
+  </si>
+  <si>
+    <t>Could you imagine if Ahsoka was just 8 episodes of Ezra and Ahsoka/Sabine swapping places?</t>
+  </si>
+  <si>
+    <t>Sounds like the plot of The Marvels but with Rebel characters</t>
+  </si>
+  <si>
+    <t>That sounds like something David Fincher would do</t>
+  </si>
+  <si>
+    <t>Ghost Anakin: AHSOOOOOOKAAAA! I’m haunting you.</t>
+  </si>
+  <si>
+    <t>Ahsoka about to pull a Cade Skywalker and smoke them sticks</t>
+  </si>
+  <si>
+    <t>Ahsoka: I’M NOT CRAZY! YOU’RE CRAZY! ESPECIALLY YOU, ANAKIN!
+Ghost Anakin: Eeeeey…!</t>
+  </si>
+  <si>
+    <t>Who you gonna call? GHOST SKYGUY</t>
+  </si>
+  <si>
+    <t>Ahso-soka-soka! Sososososoka!</t>
+  </si>
+  <si>
+    <t>I'm imagining Ahsoka chasing Ghost Anakin around with a proton pack while Anakin taunts her</t>
+  </si>
+  <si>
+    <t>And I’m out of Ghost Nappa quotes that would work.</t>
+  </si>
+  <si>
+    <t>Got any Ghostbusters ones?</t>
+  </si>
+  <si>
+    <t>Nah, I was basically running on Ghost Nappa bits.</t>
+  </si>
+  <si>
+    <t>Don't you have a son you can go bother?
+He's always busy besides you were always like a daughter to me
+Don't you have an actual daughter!
+Yeah but I kind of blew up her planet and tortured her boyfriend
+Mmmm do you really think you're in the position to give me advice considering how many bad life decisions you made
+We learn from our mistakes?
+Really though? Like did you ever do that ever?</t>
+  </si>
+  <si>
+    <t>So like Hit Monkey, but Star Wars? I'd watch it.</t>
+  </si>
+  <si>
+    <t>I’d love this tbf</t>
+  </si>
+  <si>
+    <t>I'd love a show like that. Even had an idea for one based around a similar concept.</t>
+  </si>
+  <si>
+    <t>We need the dark Anakin story ????</t>
+  </si>
+  <si>
+    <t>Watch: Episode 3</t>
+  </si>
+  <si>
+    <t>Basically v and Johnny silverhand</t>
+  </si>
+  <si>
+    <t>Ahsoka walks near tree.
+Anikan: BOO! Gotcha snips!
+Ahsoka walks down hallway approaches corner.
+Anikan: BOO! Gotcha snips!
+Ahsoka enters her ship
+Anikan: BOO! Gotcha snips!
+Ahsoka is taking a dump.
+Anikan: BOO! Gotcha snips!
+Best comedy in star wars history.</t>
+  </si>
+  <si>
+    <t>Anakin: Obi-Wan, hey Obi-Wan! Watch this!
+Obi-Wan: Again? Shouldn't you be helping your kids rebuild the galaxy?
+Anakin: They've got that handled, this'll be hilarious! Come on!</t>
+  </si>
+  <si>
+    <t>And now the hunt truly begins</t>
+  </si>
+  <si>
+    <t>Just Ahsoka running from nobody to everyone else</t>
+  </si>
+  <si>
+    <t>This is what I expect the conversation will be.</t>
+  </si>
+  <si>
+    <t>Just loving the idea of a buddy cop style show with Ashoka and the ghost of Anakin that only she can see investigating crimes throughout the outer rim</t>
+  </si>
+  <si>
+    <t>Columbo Skywalker: Oh, One More Thing..</t>
+  </si>
+  <si>
+    <t>Cameo of Liam Neeson subbing in when Anakin has to leave for a ghost-Dentist appointment he booked a few months ago. He can’t miss that ghost-teeth cleaning again.</t>
+  </si>
+  <si>
+    <t>He's gotta look his best</t>
+  </si>
+  <si>
+    <t>They should do a Star Wars show called "Force Ghosts" just to bring all of our favorite Jedi back together for a wholesome family comedy. Luke gets frustrated trying to get those power converters, Leia tells him to try and fix the moisture vaporators, and then Yoda jumps in with.....</t>
+  </si>
+  <si>
+    <t>What an upgrade</t>
+  </si>
+  <si>
+    <t>Not haunting, but straight trolling.</t>
+  </si>
+  <si>
+    <t>“Alright, keep your secrets.”</t>
+  </si>
+  <si>
+    <t>If you watch the Not Obi-wan channel on YouTube, itâ€™s Obi, force ghost Qui-gonn, and Anakin watching Star Wars stuff</t>
+  </si>
+  <si>
+    <t>This is exactly what I predicted/wanted too. I donâ€™t hate what they did, but I wish we got more PTSD Obi-Wan memories/visions/nightmares vs full on adventure.</t>
+  </si>
+  <si>
+    <t>If Disney wasnâ€™t the owner of Star Wars we wouldâ€™ve gotten a better show overallâ€¦</t>
+  </si>
+  <si>
+    <t>It wouldâ€™ve been good if people gave Solo a chance. Kenobi was a movie originally but because people didnâ€™t give Solo a chance without Ford despite it being a decent movie, they decided to scrap the movie idea</t>
+  </si>
+  <si>
+    <t>Iâ€™m still mad you lied to get on the Citadel mission Snips. Donâ€™t make me get Ploâ€™s ghost and talk it out</t>
+  </si>
+  <si>
+    <t>I would give a lot to see Ploâ€™s ghost. Except he didnâ€™t die. #PloEscapedAtTheLastMinute</t>
+  </si>
+  <si>
+    <t>â€œIs that what this is about?â€</t>
+  </si>
+  <si>
+    <t>If they leaned into it really hard then yeah. Just scenes of Ahsoka doing normal day-to-day things and Anakins ghost just standing next to her the whole time making passive aggressive comments the whole time. Iâ€™d watch that</t>
+  </si>
+  <si>
+    <t>lmao yeah, also I watched one of the episodes of them reacting and obiwan had to drug qui to not let him see anakin being vader ðŸ’€</t>
+  </si>
+  <si>
+    <t>Just like breaking plates, turning lights on and off, and opening cupboards. But heâ€™s still fully visible with a blue glow so he just looks like an asshole.</t>
+  </si>
+  <si>
+    <t>My theory is that Filioni keeps connecting the dots and Anakin also starts popping in on Luke and teasing him, so much so that he cut himself off from the force. â€œGosh dad, I KNOW FORM 3â€ - Luke â€œIncorrectâ€ - Force Ghost Anakin</t>
+  </si>
+  <si>
+    <t>Iâ€™m hoping Ahsoka and Sabine get back to their galaxy by Anakin guiding them through the world between worlds and they just pop out and land on Luke having breakfast. â€œDamn it Dad not again!â€</t>
+  </si>
+  <si>
+    <t>â€œAnakin, go away, I need privacy to go to the bathroom.â€
+â€œIncorrect.â€</t>
+  </si>
+  <si>
+    <t>Ghost Anakin: AHSOOOOOOKAAAA! Iâ€™m haunting you.</t>
+  </si>
+  <si>
+    <t>Ahsoka: Iâ€™M NOT CRAZY! YOUâ€™RE CRAZY! ESPECIALLY YOU, ANAKIN!
+Ghost Anakin: Eeeeeyâ€¦!</t>
+  </si>
+  <si>
+    <t>And Iâ€™m out of Ghost Nappa quotes that would work.</t>
+  </si>
+  <si>
+    <t>Iâ€™d love this tbf</t>
+  </si>
+  <si>
+    <t>We need the dark Anakin story ðŸ¤ŒðŸ½</t>
+  </si>
+  <si>
+    <t>Cameo of Liam Neeson subbing in when Anakin has to leave for a ghost-Dentist appointment he booked a few months ago. He canâ€™t miss that ghost-teeth cleaning again.</t>
+  </si>
+  <si>
+    <t>â€œAlright, keep your secrets.â€</t>
+  </si>
+  <si>
+    <t>Very Negative</t>
   </si>
   <si>
     <t>Neutral</t>
@@ -106,10 +424,10 @@
     <t>Positive</t>
   </si>
   <si>
+    <t>Very Positive</t>
+  </si>
+  <si>
     <t>Negative</t>
-  </si>
-  <si>
-    <t>Very Negative</t>
   </si>
 </sst>
 </file>
@@ -448,9 +766,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -459,10 +777,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>120</v>
       </c>
       <c r="C1">
-        <v>0.7</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -470,10 +788,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>121</v>
       </c>
       <c r="C2">
-        <v>0.59</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -481,10 +799,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>121</v>
       </c>
       <c r="C3">
-        <v>0.47</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -492,10 +810,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>121</v>
       </c>
       <c r="C4">
-        <v>0.63</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -503,10 +821,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>121</v>
       </c>
       <c r="C5">
-        <v>0.93</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -514,10 +832,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>122</v>
       </c>
       <c r="C6">
-        <v>0.97</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -525,10 +843,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>121</v>
       </c>
       <c r="C7">
-        <v>0.47</v>
+        <v>0.63</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -536,10 +854,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>120</v>
       </c>
       <c r="C8">
-        <v>0.52</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -547,10 +865,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>121</v>
       </c>
       <c r="C9">
-        <v>0.56999999999999995</v>
+        <v>0.77</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -558,10 +876,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>121</v>
       </c>
       <c r="C10">
-        <v>0.54</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -569,10 +887,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>123</v>
       </c>
       <c r="C11">
-        <v>0.48</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -580,10 +898,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>122</v>
       </c>
       <c r="C12">
-        <v>0.85</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -591,10 +909,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>121</v>
       </c>
       <c r="C13">
-        <v>0.86</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -602,10 +920,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>121</v>
       </c>
       <c r="C14">
-        <v>0.69</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -613,10 +931,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>124</v>
       </c>
       <c r="C15">
-        <v>0.62</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -624,10 +942,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>121</v>
       </c>
       <c r="C16">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -635,10 +953,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>121</v>
       </c>
       <c r="C17">
-        <v>0.32</v>
+        <v>0.87</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -646,10 +964,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>121</v>
       </c>
       <c r="C18">
-        <v>0.82</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -657,219 +975,1401 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>121</v>
       </c>
       <c r="C19">
-        <v>0.92</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>122</v>
       </c>
       <c r="C20">
-        <v>0.7</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>121</v>
+      </c>
+      <c r="C21">
         <v>1</v>
-      </c>
-      <c r="B21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21">
-        <v>0.59</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>121</v>
       </c>
       <c r="C22">
-        <v>0.53</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>121</v>
       </c>
       <c r="C23">
-        <v>0.53</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>121</v>
       </c>
       <c r="C24">
-        <v>0.93</v>
+        <v>0.69</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
+        <v>121</v>
       </c>
       <c r="C25">
-        <v>0.97</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>121</v>
       </c>
       <c r="C26">
-        <v>0.46</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>121</v>
       </c>
       <c r="C27">
-        <v>0.52</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>26</v>
+        <v>121</v>
       </c>
       <c r="C28">
-        <v>0.49</v>
+        <v>0.83</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>26</v>
+        <v>121</v>
       </c>
       <c r="C29">
-        <v>0.57999999999999996</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>26</v>
+        <v>121</v>
       </c>
       <c r="C30">
-        <v>0.48</v>
+        <v>0.69</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>26</v>
+        <v>121</v>
       </c>
       <c r="C31">
-        <v>0.85</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>26</v>
+        <v>121</v>
       </c>
       <c r="C32">
-        <v>0.86</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>26</v>
+        <v>121</v>
       </c>
       <c r="C33">
-        <v>0.69</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>29</v>
+        <v>122</v>
       </c>
       <c r="C34">
-        <v>0.67</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>29</v>
+        <v>121</v>
       </c>
       <c r="C35">
-        <v>0.8</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>27</v>
+        <v>121</v>
       </c>
       <c r="C36">
-        <v>0.32</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>28</v>
+        <v>121</v>
       </c>
       <c r="C37">
-        <v>0.82</v>
+        <v>0.77</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="B38" t="s">
+        <v>124</v>
+      </c>
+      <c r="C38">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>123</v>
+      </c>
+      <c r="C39">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>121</v>
+      </c>
+      <c r="C40">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>121</v>
+      </c>
+      <c r="C41">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>122</v>
+      </c>
+      <c r="C42">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>121</v>
+      </c>
+      <c r="C43">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>121</v>
+      </c>
+      <c r="C44">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>121</v>
+      </c>
+      <c r="C45">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>123</v>
+      </c>
+      <c r="C46">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>121</v>
+      </c>
+      <c r="C47">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>122</v>
+      </c>
+      <c r="C48">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>122</v>
+      </c>
+      <c r="C49">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>121</v>
+      </c>
+      <c r="C50">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>121</v>
+      </c>
+      <c r="C51">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>122</v>
+      </c>
+      <c r="C52">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>122</v>
+      </c>
+      <c r="C53">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>121</v>
+      </c>
+      <c r="C54">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>124</v>
+      </c>
+      <c r="C55">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>121</v>
+      </c>
+      <c r="C56">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>121</v>
+      </c>
+      <c r="C57">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>121</v>
+      </c>
+      <c r="C58">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>121</v>
+      </c>
+      <c r="C59">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>121</v>
+      </c>
+      <c r="C60">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>122</v>
+      </c>
+      <c r="C61">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>122</v>
+      </c>
+      <c r="C62">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>124</v>
+      </c>
+      <c r="C63">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>121</v>
+      </c>
+      <c r="C64">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>122</v>
+      </c>
+      <c r="C65">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>121</v>
+      </c>
+      <c r="C66">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>121</v>
+      </c>
+      <c r="C67">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>121</v>
+      </c>
+      <c r="C68">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>124</v>
+      </c>
+      <c r="C69">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>121</v>
+      </c>
+      <c r="C70">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>120</v>
+      </c>
+      <c r="C71">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>122</v>
+      </c>
+      <c r="C72">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>120</v>
+      </c>
+      <c r="C73">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>121</v>
+      </c>
+      <c r="C74">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>121</v>
+      </c>
+      <c r="C75">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>121</v>
+      </c>
+      <c r="C76">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>121</v>
+      </c>
+      <c r="C77">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>124</v>
+      </c>
+      <c r="C78">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>120</v>
+      </c>
+      <c r="C79">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>121</v>
+      </c>
+      <c r="C80">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>123</v>
+      </c>
+      <c r="C81">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>121</v>
+      </c>
+      <c r="C82">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>123</v>
+      </c>
+      <c r="C83">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>122</v>
+      </c>
+      <c r="C84">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>121</v>
+      </c>
+      <c r="C85">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>121</v>
+      </c>
+      <c r="C86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
+        <v>121</v>
+      </c>
+      <c r="C87">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>87</v>
+      </c>
+      <c r="B88" t="s">
+        <v>122</v>
+      </c>
+      <c r="C88">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>88</v>
+      </c>
+      <c r="B89" t="s">
+        <v>121</v>
+      </c>
+      <c r="C89">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>89</v>
+      </c>
+      <c r="B90" t="s">
+        <v>121</v>
+      </c>
+      <c r="C90">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>90</v>
+      </c>
+      <c r="B91" t="s">
+        <v>121</v>
+      </c>
+      <c r="C91">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>91</v>
+      </c>
+      <c r="B92" t="s">
+        <v>121</v>
+      </c>
+      <c r="C92">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>92</v>
+      </c>
+      <c r="B93" t="s">
+        <v>121</v>
+      </c>
+      <c r="C93">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>93</v>
+      </c>
+      <c r="B94" t="s">
+        <v>121</v>
+      </c>
+      <c r="C94">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>94</v>
+      </c>
+      <c r="B95" t="s">
+        <v>121</v>
+      </c>
+      <c r="C95">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>95</v>
+      </c>
+      <c r="B96" t="s">
+        <v>121</v>
+      </c>
+      <c r="C96">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>96</v>
+      </c>
+      <c r="B97" t="s">
+        <v>124</v>
+      </c>
+      <c r="C97">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>97</v>
+      </c>
+      <c r="B98" t="s">
+        <v>122</v>
+      </c>
+      <c r="C98">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>98</v>
+      </c>
+      <c r="B99" t="s">
+        <v>121</v>
+      </c>
+      <c r="C99">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>99</v>
+      </c>
+      <c r="B100" t="s">
+        <v>121</v>
+      </c>
+      <c r="C100">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
         <v>26</v>
       </c>
-      <c r="C38">
-        <v>0.92</v>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>